<commit_message>
its going well bois
</commit_message>
<xml_diff>
--- a/CHP2/heat_demand.xlsx
+++ b/CHP2/heat_demand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheikh M Ahmed\modelling_MCDM\CHP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B40C31-52D2-423C-B189-1B05CEBADBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF5E96D-6AEB-4896-8823-30D7D23290CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{5524CA32-E132-410D-B865-513BEFDAB590}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,13 +426,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>505</v>
+        <f ca="1">RANDBETWEEN(400,550)</f>
+        <v>526</v>
       </c>
       <c r="C2">
-        <v>600</v>
+        <f ca="1">RANDBETWEEN(500,600)</f>
+        <v>539</v>
       </c>
       <c r="D2">
-        <v>200</v>
+        <f ca="1">RANDBETWEEN(180,220)</f>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -440,13 +443,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>520</v>
+        <f t="shared" ref="B3:B9" ca="1" si="0">RANDBETWEEN(400,550)</f>
+        <v>525</v>
       </c>
       <c r="C3">
-        <v>600</v>
+        <f t="shared" ref="C3:C8" ca="1" si="1">RANDBETWEEN(500,600)</f>
+        <v>536</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <f t="shared" ref="D3:D25" ca="1" si="2">RANDBETWEEN(180,220)</f>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -454,13 +460,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>560</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>457</v>
       </c>
       <c r="C4">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>555</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -468,13 +477,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>505</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>471</v>
       </c>
       <c r="C5">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>569</v>
       </c>
       <c r="D5">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -482,13 +494,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>550</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>405</v>
       </c>
       <c r="C6">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>592</v>
       </c>
       <c r="D6">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -496,13 +511,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>520</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>549</v>
       </c>
       <c r="C7">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>596</v>
       </c>
       <c r="D7">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -510,13 +528,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>510</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>504</v>
       </c>
       <c r="C8">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>555</v>
       </c>
       <c r="D8">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -524,13 +545,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>800</v>
+        <f ca="1">RANDBETWEEN(700,900)</f>
+        <v>762</v>
       </c>
       <c r="C9">
-        <v>1800</v>
+        <f ca="1">RANDBETWEEN(1800,2400)</f>
+        <v>2118</v>
       </c>
       <c r="D9">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -538,13 +562,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>810</v>
+        <f t="shared" ref="B10:B17" ca="1" si="3">RANDBETWEEN(700,900)</f>
+        <v>783</v>
       </c>
       <c r="C10">
-        <v>1900</v>
+        <f t="shared" ref="C10:C21" ca="1" si="4">RANDBETWEEN(1800,2400)</f>
+        <v>2134</v>
       </c>
       <c r="D10">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -552,13 +579,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>820</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>871</v>
       </c>
       <c r="C11">
-        <v>1800</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2378</v>
       </c>
       <c r="D11">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -566,13 +596,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>810</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>719</v>
       </c>
       <c r="C12">
-        <v>1600</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2060</v>
       </c>
       <c r="D12">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -580,13 +613,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>805</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>854</v>
       </c>
       <c r="C13">
-        <v>1500</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1958</v>
       </c>
       <c r="D13">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -594,13 +630,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>800</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>782</v>
       </c>
       <c r="C14">
-        <v>1900</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2091</v>
       </c>
       <c r="D14">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -608,13 +647,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>790</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>760</v>
       </c>
       <c r="C15">
-        <v>1950</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1978</v>
       </c>
       <c r="D15">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -622,13 +664,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>810</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>882</v>
       </c>
       <c r="C16">
-        <v>1920</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2279</v>
       </c>
       <c r="D16">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -636,13 +681,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>800</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>821</v>
       </c>
       <c r="C17">
-        <v>1960</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1907</v>
       </c>
       <c r="D17">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -650,13 +698,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>505</v>
+        <f ca="1">RANDBETWEEN(400,550)</f>
+        <v>461</v>
       </c>
       <c r="C18">
-        <v>1500</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2178</v>
       </c>
       <c r="D18">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -664,13 +715,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>520</v>
+        <f t="shared" ref="B19:B25" ca="1" si="5">RANDBETWEEN(400,550)</f>
+        <v>492</v>
       </c>
       <c r="C19">
-        <v>1900</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1851</v>
       </c>
       <c r="D19">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,13 +732,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>560</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>498</v>
       </c>
       <c r="C20">
-        <v>1950</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1839</v>
       </c>
       <c r="D20">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,13 +749,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>505</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>410</v>
       </c>
       <c r="C21">
-        <v>1920</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2134</v>
       </c>
       <c r="D21">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -706,13 +766,16 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>550</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>408</v>
       </c>
       <c r="C22">
-        <v>600</v>
+        <f t="shared" ref="C22:C25" ca="1" si="6">RANDBETWEEN(500,600)</f>
+        <v>561</v>
       </c>
       <c r="D22">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -720,13 +783,16 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>520</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>483</v>
       </c>
       <c r="C23">
-        <v>600</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>507</v>
       </c>
       <c r="D23">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -734,13 +800,16 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>510</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>419</v>
       </c>
       <c r="C24">
-        <v>600</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>512</v>
       </c>
       <c r="D24">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,13 +817,16 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>520</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>426</v>
       </c>
       <c r="C25">
-        <v>600</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>512</v>
       </c>
       <c r="D25">
-        <v>200</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no problems as of yet
</commit_message>
<xml_diff>
--- a/CHP2/heat_demand.xlsx
+++ b/CHP2/heat_demand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheikh M Ahmed\modelling_MCDM\CHP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF5E96D-6AEB-4896-8823-30D7D23290CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA897E77-FFE7-47C2-8791-A627CFE4779E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{5524CA32-E132-410D-B865-513BEFDAB590}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>elec</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>cool</t>
+  </si>
+  <si>
+    <t>elec_hard</t>
+  </si>
+  <si>
+    <t>heat_hard</t>
+  </si>
+  <si>
+    <t>carbon</t>
   </si>
 </sst>
 </file>
@@ -399,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D915BB96-A88E-4797-BAC2-270B960E39C0}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -420,413 +429,686 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(400,550)</f>
-        <v>526</v>
+        <v>404</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(500,600)</f>
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(180,220)</f>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(200, 2000)</f>
+        <v>1527</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(200,4000)</f>
+        <v>1058</v>
+      </c>
+      <c r="G2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B9" ca="1" si="0">RANDBETWEEN(400,550)</f>
-        <v>525</v>
+        <f t="shared" ref="B3:B8" ca="1" si="0">RANDBETWEEN(400,550)</f>
+        <v>517</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="1">RANDBETWEEN(500,600)</f>
-        <v>536</v>
+        <v>545</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D25" ca="1" si="2">RANDBETWEEN(180,220)</f>
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E25" ca="1" si="3">RANDBETWEEN(200, 2000)</f>
+        <v>1412</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F25" ca="1" si="4">RANDBETWEEN(200,4000)</f>
+        <v>1244</v>
+      </c>
+      <c r="G3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>457</v>
+        <v>472</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="2"/>
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="3"/>
+        <v>1030</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="4"/>
+        <v>1870</v>
+      </c>
+      <c r="G4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>471</v>
+        <v>523</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>569</v>
+        <v>538</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="2"/>
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="3"/>
+        <v>1604</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="4"/>
+        <v>2773</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>405</v>
+        <v>426</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>592</v>
+        <v>515</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="3"/>
+        <v>1284</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="4"/>
+        <v>707</v>
+      </c>
+      <c r="G6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>549</v>
+        <v>465</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>596</v>
+        <v>524</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="3"/>
+        <v>1281</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="4"/>
+        <v>1541</v>
+      </c>
+      <c r="G7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>504</v>
+        <v>523</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>555</v>
+        <v>514</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
         <v>210</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <f t="shared" ca="1" si="3"/>
+        <v>974</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="4"/>
+        <v>3099</v>
+      </c>
+      <c r="G8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <f ca="1">RANDBETWEEN(700,900)</f>
-        <v>762</v>
+        <v>703</v>
       </c>
       <c r="C9">
         <f ca="1">RANDBETWEEN(1800,2400)</f>
-        <v>2118</v>
+        <v>1906</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="3"/>
+        <v>998</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="4"/>
+        <v>2461</v>
+      </c>
+      <c r="G9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10:B17" ca="1" si="3">RANDBETWEEN(700,900)</f>
-        <v>783</v>
+        <f t="shared" ref="B10:B17" ca="1" si="5">RANDBETWEEN(700,900)</f>
+        <v>894</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:C21" ca="1" si="4">RANDBETWEEN(1800,2400)</f>
-        <v>2134</v>
+        <f t="shared" ref="C10:C21" ca="1" si="6">RANDBETWEEN(1800,2400)</f>
+        <v>2000</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="2"/>
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="3"/>
+        <v>790</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="4"/>
+        <v>3719</v>
+      </c>
+      <c r="G10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="3"/>
-        <v>871</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>829</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="4"/>
-        <v>2378</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1809</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="2"/>
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="3"/>
+        <v>834</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="4"/>
+        <v>3642</v>
+      </c>
+      <c r="G11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" ca="1" si="3"/>
-        <v>719</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>756</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="4"/>
-        <v>2060</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2329</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="3"/>
+        <v>219</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="4"/>
+        <v>1034</v>
+      </c>
+      <c r="G12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="3"/>
-        <v>854</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>870</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="4"/>
-        <v>1958</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2065</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="2"/>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="3"/>
+        <v>1683</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="4"/>
+        <v>2960</v>
+      </c>
+      <c r="G13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="3"/>
-        <v>782</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>863</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="4"/>
-        <v>2091</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1829</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="2"/>
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="3"/>
+        <v>1858</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="4"/>
+        <v>3621</v>
+      </c>
+      <c r="G14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="3"/>
-        <v>760</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>835</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="4"/>
-        <v>1978</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1973</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="2"/>
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="3"/>
+        <v>580</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="4"/>
+        <v>3521</v>
+      </c>
+      <c r="G15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="3"/>
-        <v>882</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>890</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="4"/>
-        <v>2279</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2110</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="2"/>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="3"/>
+        <v>1579</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="4"/>
+        <v>1439</v>
+      </c>
+      <c r="G16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" ca="1" si="3"/>
-        <v>821</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>872</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="4"/>
-        <v>1907</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2240</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="2"/>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="3"/>
+        <v>736</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="4"/>
+        <v>3234</v>
+      </c>
+      <c r="G17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <f ca="1">RANDBETWEEN(400,550)</f>
-        <v>461</v>
+        <v>530</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="4"/>
-        <v>2178</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2304</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="2"/>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="4"/>
+        <v>1063</v>
+      </c>
+      <c r="G18">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B25" ca="1" si="5">RANDBETWEEN(400,550)</f>
-        <v>492</v>
+        <f t="shared" ref="B19:B25" ca="1" si="7">RANDBETWEEN(400,550)</f>
+        <v>500</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="4"/>
-        <v>1851</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1895</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="2"/>
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="3"/>
+        <v>1639</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="4"/>
+        <v>2304</v>
+      </c>
+      <c r="G19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="5"/>
-        <v>498</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>442</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="4"/>
-        <v>1839</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1990</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="2"/>
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="3"/>
+        <v>1446</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="4"/>
+        <v>3402</v>
+      </c>
+      <c r="G20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" ca="1" si="5"/>
-        <v>410</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>463</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="4"/>
-        <v>2134</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2050</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="2"/>
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="3"/>
+        <v>1361</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="4"/>
+        <v>1765</v>
+      </c>
+      <c r="G21">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="5"/>
-        <v>408</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>505</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:C25" ca="1" si="6">RANDBETWEEN(500,600)</f>
-        <v>561</v>
+        <f t="shared" ref="C22:C25" ca="1" si="8">RANDBETWEEN(500,600)</f>
+        <v>505</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="2"/>
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="3"/>
+        <v>1743</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="4"/>
+        <v>684</v>
+      </c>
+      <c r="G22">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="5"/>
-        <v>483</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>416</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="6"/>
-        <v>507</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>599</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="2"/>
-        <v>189</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="3"/>
+        <v>1700</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="4"/>
+        <v>904</v>
+      </c>
+      <c r="G23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="5"/>
-        <v>419</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>445</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="6"/>
-        <v>512</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>590</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="2"/>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="3"/>
+        <v>1183</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="4"/>
+        <v>3562</v>
+      </c>
+      <c r="G24">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="5"/>
-        <v>426</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>479</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="6"/>
-        <v>512</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>563</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="2"/>
-        <v>206</v>
+        <v>219</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="3"/>
+        <v>1342</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ca="1" si="4"/>
+        <v>2484</v>
+      </c>
+      <c r="G25">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>